<commit_message>
Casos de Prueba de Carrera
</commit_message>
<xml_diff>
--- a/2 - Analisis y Diseño/Casos de Prueba/CP - Correlatividades.xlsx
+++ b/2 - Analisis y Diseño/Casos de Prueba/CP - Correlatividades.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="15480" windowHeight="10620" tabRatio="627" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="15480" windowHeight="10620" tabRatio="627"/>
   </bookViews>
   <sheets>
     <sheet name="End2End Positivos" sheetId="3" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="59">
   <si>
     <t>Datos de prueba</t>
   </si>
@@ -169,30 +169,6 @@
   </si>
   <si>
     <t>Confirma Eliminar</t>
-  </si>
-  <si>
-    <t>Editar Correlatividad</t>
-  </si>
-  <si>
-    <t>Editar</t>
-  </si>
-  <si>
-    <t>Redirige a la vista de Edición de Correlatividades.</t>
-  </si>
-  <si>
-    <t>Modificar los datos necesarios</t>
-  </si>
-  <si>
-    <t>Actualizar</t>
-  </si>
-  <si>
-    <t>Redirige a la vista de la Correlatividad con los datos Actualizados.</t>
-  </si>
-  <si>
-    <t>Modificación</t>
-  </si>
-  <si>
-    <t>Alta/Modificación</t>
   </si>
   <si>
     <t>Correlatividad con Materias Diferente Plan</t>
@@ -1065,81 +1041,84 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="14" xfId="216" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="12" xfId="216" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="23" xfId="216" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="6" xfId="216" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="20" xfId="216" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="7" xfId="216" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="15" xfId="216" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="21" xfId="216" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="23" xfId="216" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="14" xfId="216" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="12" xfId="216" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="15" xfId="216" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="21" xfId="216" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="6" xfId="216" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="20" xfId="216" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="23" xfId="216" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="7" xfId="216" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="23" xfId="216" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1149,10 +1128,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1678,13 +1654,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="5" ySplit="11" topLeftCell="F12" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12:H16"/>
+      <selection pane="bottomRight" activeCell="D27" sqref="D27:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1753,13 +1729,13 @@
     </row>
     <row r="3" spans="1:18" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="14"/>
@@ -1797,8 +1773,8 @@
         <v>11</v>
       </c>
       <c r="C5" s="17">
-        <f>COUNTIF(A11:A587,"&gt;0")</f>
-        <v>3</v>
+        <f>COUNTIF(A11:A582,"&gt;0")</f>
+        <v>2</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>13</v>
@@ -1823,7 +1799,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="19" t="e">
-        <f>SUM(P9:P587)/C5</f>
+        <f>SUM(P9:P582)/C5</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D6" s="18" t="s">
@@ -1849,7 +1825,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="19" t="e">
-        <f>SUM(Q9:Q587)/C5</f>
+        <f>SUM(Q9:Q582)/C5</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D7" s="18" t="s">
@@ -1990,16 +1966,16 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="59">
+      <c r="A12" s="69">
         <v>1</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="72" t="s">
         <v>32</v>
       </c>
       <c r="E12" s="12">
@@ -2008,7 +1984,7 @@
       <c r="F12" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="71" t="s">
+      <c r="G12" s="48" t="s">
         <v>34</v>
       </c>
       <c r="H12" s="24" t="s">
@@ -2023,43 +1999,43 @@
         <f t="shared" ref="K12" si="1">+IF(I12="OK",1,0)</f>
         <v>0</v>
       </c>
-      <c r="L12" s="51">
+      <c r="L12" s="55">
         <f>+(COUNTIF(J12:J16,1))</f>
         <v>0</v>
       </c>
-      <c r="M12" s="49">
+      <c r="M12" s="52">
         <f>+COUNT(E12:E16)</f>
         <v>5</v>
       </c>
-      <c r="N12" s="51">
+      <c r="N12" s="55">
         <f>+(COUNTIF(K12:K16,1))</f>
         <v>0</v>
       </c>
-      <c r="O12" s="53">
-        <v>0</v>
-      </c>
-      <c r="P12" s="57">
+      <c r="O12" s="58">
+        <v>0</v>
+      </c>
+      <c r="P12" s="61">
         <f>+L12/M12</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="55">
+      <c r="Q12" s="64">
         <f>+N12/M12</f>
         <v>0</v>
       </c>
       <c r="R12" s="31"/>
     </row>
     <row r="13" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="62"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="71"/>
       <c r="E13" s="1">
         <v>2</v>
       </c>
       <c r="F13" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="71" t="s">
+      <c r="G13" s="48" t="s">
         <v>34</v>
       </c>
       <c r="H13" s="11" t="s">
@@ -2068,19 +2044,19 @@
       <c r="I13" s="4"/>
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="54"/>
-      <c r="P13" s="58"/>
-      <c r="Q13" s="56"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="65"/>
       <c r="R13" s="29"/>
     </row>
     <row r="14" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="60"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="62"/>
+      <c r="A14" s="70"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="71"/>
       <c r="E14" s="1">
         <v>3</v>
       </c>
@@ -2094,45 +2070,45 @@
       <c r="I14" s="4"/>
       <c r="J14" s="39"/>
       <c r="K14" s="39"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="65"/>
       <c r="R14" s="29"/>
     </row>
     <row r="15" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="60"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="62"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="71"/>
       <c r="E15" s="1">
         <v>4</v>
       </c>
       <c r="F15" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="72" t="s">
+      <c r="G15" s="49" t="s">
         <v>37</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="4"/>
       <c r="J15" s="39"/>
       <c r="K15" s="39"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="54"/>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="65"/>
       <c r="R15" s="29"/>
     </row>
     <row r="16" spans="1:18" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="62"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="71"/>
       <c r="E16" s="1">
         <v>5</v>
       </c>
@@ -2148,25 +2124,25 @@
       <c r="I16" s="4"/>
       <c r="J16" s="39"/>
       <c r="K16" s="39"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="52"/>
-      <c r="O16" s="54"/>
-      <c r="P16" s="58"/>
-      <c r="Q16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="59"/>
+      <c r="P16" s="62"/>
+      <c r="Q16" s="65"/>
       <c r="R16" s="29"/>
     </row>
     <row r="17" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="59">
+      <c r="A17" s="69">
         <v>2</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="61" t="s">
+      <c r="D17" s="72" t="s">
         <v>44</v>
       </c>
       <c r="E17" s="12">
@@ -2175,7 +2151,7 @@
       <c r="F17" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="71" t="s">
+      <c r="G17" s="48" t="s">
         <v>34</v>
       </c>
       <c r="H17" s="24" t="s">
@@ -2190,43 +2166,43 @@
         <f t="shared" ref="K17" si="3">+IF(I17="OK",1,0)</f>
         <v>0</v>
       </c>
-      <c r="L17" s="51">
+      <c r="L17" s="55">
         <f>+(COUNTIF(J17:J20,1))</f>
         <v>0</v>
       </c>
-      <c r="M17" s="49">
+      <c r="M17" s="52">
         <f>+COUNT(E17:E20)</f>
         <v>4</v>
       </c>
-      <c r="N17" s="51">
+      <c r="N17" s="55">
         <f>+(COUNTIF(K17:K20,1))</f>
         <v>0</v>
       </c>
-      <c r="O17" s="53">
-        <v>0</v>
-      </c>
-      <c r="P17" s="57">
+      <c r="O17" s="58">
+        <v>0</v>
+      </c>
+      <c r="P17" s="61">
         <f>+L17/M17</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="55">
+      <c r="Q17" s="64">
         <f>+N17/M17</f>
         <v>0</v>
       </c>
       <c r="R17" s="31"/>
     </row>
     <row r="18" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="60"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="62"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="1">
         <v>2</v>
       </c>
       <c r="F18" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="71" t="s">
+      <c r="G18" s="48" t="s">
         <v>34</v>
       </c>
       <c r="H18" s="11" t="s">
@@ -2235,19 +2211,19 @@
       <c r="I18" s="4"/>
       <c r="J18" s="39"/>
       <c r="K18" s="39"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="52"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="58"/>
-      <c r="Q18" s="56"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="59"/>
+      <c r="P18" s="62"/>
+      <c r="Q18" s="65"/>
       <c r="R18" s="29"/>
     </row>
     <row r="19" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="60"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="62"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="1">
         <v>3</v>
       </c>
@@ -2263,26 +2239,26 @@
       <c r="I19" s="4"/>
       <c r="J19" s="39"/>
       <c r="K19" s="39"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="52"/>
-      <c r="O19" s="54"/>
-      <c r="P19" s="58"/>
-      <c r="Q19" s="56"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="65"/>
       <c r="R19" s="29"/>
     </row>
     <row r="20" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="60"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="62"/>
+      <c r="A20" s="70"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="71"/>
       <c r="E20" s="1">
         <v>4</v>
       </c>
       <c r="F20" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="72" t="s">
+      <c r="G20" s="49" t="s">
         <v>40</v>
       </c>
       <c r="H20" s="11" t="s">
@@ -2291,39 +2267,23 @@
       <c r="I20" s="4"/>
       <c r="J20" s="39"/>
       <c r="K20" s="39"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="52"/>
-      <c r="O20" s="54"/>
-      <c r="P20" s="58"/>
-      <c r="Q20" s="56"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="59"/>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="65"/>
       <c r="R20" s="29"/>
     </row>
-    <row r="21" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="59">
-        <v>3</v>
-      </c>
-      <c r="B21" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="12">
-        <v>1</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="24" t="s">
-        <v>35</v>
-      </c>
+    <row r="21" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="69"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="24"/>
       <c r="I21" s="27"/>
       <c r="J21" s="30">
         <f t="shared" ref="J21" si="4">+IF(I21="OK",1,(IF(I21="No Ok",1,0)))</f>
@@ -2333,484 +2293,321 @@
         <f t="shared" ref="K21" si="5">+IF(I21="OK",1,0)</f>
         <v>0</v>
       </c>
-      <c r="L21" s="51">
-        <f>+(COUNTIF(J21:J25,1))</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="49">
-        <f>+COUNT(E21:E25)</f>
-        <v>5</v>
-      </c>
-      <c r="N21" s="51">
-        <f>+(COUNTIF(K21:K25,1))</f>
-        <v>0</v>
-      </c>
-      <c r="O21" s="53">
-        <v>0</v>
-      </c>
-      <c r="P21" s="57">
+      <c r="L21" s="55">
+        <f>+(COUNTIF(J21:J26,1))</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="52">
+        <f>+COUNT(E21:E26)</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="55">
+        <f>+(COUNTIF(K21:K26,1))</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="58">
+        <v>0</v>
+      </c>
+      <c r="P21" s="61" t="e">
         <f>+L21/M21</f>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="55">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q21" s="64" t="e">
         <f>+N21/M21</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="R21" s="31"/>
     </row>
     <row r="22" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="60"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="1">
-        <v>2</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>47</v>
-      </c>
+      <c r="A22" s="70"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="11"/>
       <c r="I22" s="4"/>
       <c r="J22" s="39"/>
       <c r="K22" s="39"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="52"/>
-      <c r="O22" s="54"/>
-      <c r="P22" s="58"/>
-      <c r="Q22" s="56"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="62"/>
+      <c r="Q22" s="65"/>
       <c r="R22" s="29"/>
     </row>
     <row r="23" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="60"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="1">
-        <v>3</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="G23" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>52</v>
-      </c>
+      <c r="A23" s="70"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="11"/>
       <c r="I23" s="4"/>
       <c r="J23" s="39"/>
       <c r="K23" s="39"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="58"/>
-      <c r="Q23" s="56"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="59"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="65"/>
       <c r="R23" s="29"/>
     </row>
-    <row r="24" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="60"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="1">
-        <v>4</v>
-      </c>
-      <c r="F24" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="72" t="s">
-        <v>37</v>
-      </c>
+    <row r="24" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="70"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="28"/>
       <c r="H24" s="11"/>
       <c r="I24" s="4"/>
       <c r="J24" s="39"/>
       <c r="K24" s="39"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="54"/>
-      <c r="P24" s="58"/>
-      <c r="Q24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="59"/>
+      <c r="P24" s="62"/>
+      <c r="Q24" s="65"/>
       <c r="R24" s="29"/>
     </row>
-    <row r="25" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="60"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="1">
-        <v>5</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>55</v>
-      </c>
+    <row r="25" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="70"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="28"/>
       <c r="I25" s="4"/>
       <c r="J25" s="39"/>
       <c r="K25" s="39"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="52"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="56"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="65"/>
       <c r="R25" s="29"/>
     </row>
-    <row r="26" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="59"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="30">
-        <f t="shared" ref="J26" si="6">+IF(I26="OK",1,(IF(I26="No Ok",1,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="K26" s="30">
-        <f t="shared" ref="K26" si="7">+IF(I26="OK",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="L26" s="51">
-        <f>+(COUNTIF(J26:J31,1))</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="49">
-        <f>+COUNT(E26:E31)</f>
-        <v>0</v>
-      </c>
-      <c r="N26" s="51">
-        <f>+(COUNTIF(K26:K31,1))</f>
-        <v>0</v>
-      </c>
-      <c r="O26" s="53">
-        <v>0</v>
-      </c>
-      <c r="P26" s="57" t="e">
-        <f>+L26/M26</f>
+    <row r="26" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="71"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="66"/>
+      <c r="R26" s="44"/>
+    </row>
+    <row r="27" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="67"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="30">
+        <f t="shared" ref="J27" si="6">+IF(I27="OK",1,(IF(I27="No Ok",1,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="30">
+        <f t="shared" ref="K27" si="7">+IF(I27="OK",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="55">
+        <f>+(COUNTIF(J27:J32,1))</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="52">
+        <f>+COUNT(E27:E32)</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="55">
+        <f>+(COUNTIF(K27:K32,1))</f>
+        <v>0</v>
+      </c>
+      <c r="O27" s="58">
+        <v>0</v>
+      </c>
+      <c r="P27" s="61" t="e">
+        <f>+L27/M27</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q26" s="55" t="e">
-        <f>+N26/M26</f>
+      <c r="Q27" s="64" t="e">
+        <f>+N27/M27</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R26" s="31"/>
-    </row>
-    <row r="27" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="60"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="52"/>
-      <c r="O27" s="54"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="56"/>
-      <c r="R27" s="29"/>
-    </row>
-    <row r="28" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="60"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="62"/>
+      <c r="R27" s="31"/>
+    </row>
+    <row r="28" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="67"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
       <c r="E28" s="1"/>
       <c r="F28" s="25"/>
-      <c r="G28" s="20"/>
+      <c r="G28" s="41"/>
       <c r="H28" s="11"/>
       <c r="I28" s="4"/>
       <c r="J28" s="39"/>
       <c r="K28" s="39"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="50"/>
-      <c r="N28" s="52"/>
-      <c r="O28" s="54"/>
-      <c r="P28" s="58"/>
-      <c r="Q28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="59"/>
+      <c r="P28" s="62"/>
+      <c r="Q28" s="65"/>
       <c r="R28" s="29"/>
     </row>
-    <row r="29" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="60"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="62"/>
+    <row r="29" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="67"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="28"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="20"/>
       <c r="H29" s="11"/>
       <c r="I29" s="4"/>
       <c r="J29" s="39"/>
       <c r="K29" s="39"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="50"/>
-      <c r="N29" s="52"/>
-      <c r="O29" s="54"/>
-      <c r="P29" s="58"/>
-      <c r="Q29" s="56"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="59"/>
+      <c r="P29" s="62"/>
+      <c r="Q29" s="65"/>
       <c r="R29" s="29"/>
     </row>
-    <row r="30" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="60"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="62"/>
+    <row r="30" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="67"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="28"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="11"/>
       <c r="I30" s="4"/>
       <c r="J30" s="39"/>
       <c r="K30" s="39"/>
-      <c r="L30" s="52"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="52"/>
-      <c r="O30" s="54"/>
-      <c r="P30" s="58"/>
-      <c r="Q30" s="56"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="53"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="59"/>
+      <c r="P30" s="62"/>
+      <c r="Q30" s="65"/>
       <c r="R30" s="29"/>
     </row>
-    <row r="31" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="62"/>
-      <c r="B31" s="62"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="64"/>
-      <c r="M31" s="65"/>
-      <c r="N31" s="64"/>
-      <c r="O31" s="66"/>
-      <c r="P31" s="67"/>
-      <c r="Q31" s="68"/>
-      <c r="R31" s="44"/>
-    </row>
-    <row r="32" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="69"/>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="30">
-        <f t="shared" ref="J32" si="8">+IF(I32="OK",1,(IF(I32="No Ok",1,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="K32" s="30">
-        <f t="shared" ref="K32" si="9">+IF(I32="OK",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="L32" s="51">
-        <f>+(COUNTIF(J32:J37,1))</f>
-        <v>0</v>
-      </c>
-      <c r="M32" s="49">
-        <f>+COUNT(E32:E37)</f>
-        <v>0</v>
-      </c>
-      <c r="N32" s="51">
-        <f>+(COUNTIF(K32:K37,1))</f>
-        <v>0</v>
-      </c>
-      <c r="O32" s="53">
-        <v>0</v>
-      </c>
-      <c r="P32" s="57" t="e">
-        <f>+L32/M32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q32" s="55" t="e">
-        <f>+N32/M32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R32" s="31"/>
-    </row>
-    <row r="33" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="69"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="50"/>
-      <c r="N33" s="52"/>
-      <c r="O33" s="54"/>
-      <c r="P33" s="58"/>
-      <c r="Q33" s="56"/>
-      <c r="R33" s="29"/>
-    </row>
-    <row r="34" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="69"/>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="54"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="56"/>
-      <c r="R34" s="29"/>
-    </row>
-    <row r="35" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="69"/>
-      <c r="B35" s="69"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="52"/>
-      <c r="M35" s="50"/>
-      <c r="N35" s="52"/>
-      <c r="O35" s="54"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="56"/>
-      <c r="R35" s="29"/>
-    </row>
-    <row r="36" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="69"/>
-      <c r="B36" s="69"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="52"/>
-      <c r="M36" s="50"/>
-      <c r="N36" s="52"/>
-      <c r="O36" s="54"/>
-      <c r="P36" s="58"/>
-      <c r="Q36" s="56"/>
-      <c r="R36" s="29"/>
-    </row>
-    <row r="37" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="70"/>
-      <c r="B37" s="70"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="64"/>
-      <c r="M37" s="65"/>
-      <c r="N37" s="64"/>
-      <c r="O37" s="66"/>
-      <c r="P37" s="67"/>
-      <c r="Q37" s="68"/>
-      <c r="R37" s="44"/>
+    <row r="31" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="67"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="53"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="59"/>
+      <c r="P31" s="62"/>
+      <c r="Q31" s="65"/>
+      <c r="R31" s="29"/>
+    </row>
+    <row r="32" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="68"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="57"/>
+      <c r="M32" s="54"/>
+      <c r="N32" s="57"/>
+      <c r="O32" s="60"/>
+      <c r="P32" s="63"/>
+      <c r="Q32" s="66"/>
+      <c r="R32" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="M32:M37"/>
-    <mergeCell ref="N32:N37"/>
-    <mergeCell ref="O32:O37"/>
-    <mergeCell ref="P32:P37"/>
-    <mergeCell ref="Q32:Q37"/>
-    <mergeCell ref="L32:L37"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="C32:C37"/>
-    <mergeCell ref="D32:D37"/>
-    <mergeCell ref="M26:M31"/>
-    <mergeCell ref="N26:N31"/>
-    <mergeCell ref="O26:O31"/>
-    <mergeCell ref="P26:P31"/>
-    <mergeCell ref="Q26:Q31"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="C26:C31"/>
-    <mergeCell ref="D26:D31"/>
-    <mergeCell ref="L26:L31"/>
-    <mergeCell ref="M21:M25"/>
-    <mergeCell ref="N21:N25"/>
-    <mergeCell ref="O21:O25"/>
-    <mergeCell ref="P21:P25"/>
-    <mergeCell ref="Q21:Q25"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="L21:L25"/>
-    <mergeCell ref="M17:M20"/>
-    <mergeCell ref="N17:N20"/>
-    <mergeCell ref="O17:O20"/>
-    <mergeCell ref="P17:P20"/>
-    <mergeCell ref="Q17:Q20"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="L17:L20"/>
+  <mergeCells count="41">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="M12:M16"/>
+    <mergeCell ref="N12:N16"/>
+    <mergeCell ref="O12:O16"/>
+    <mergeCell ref="L12:L16"/>
     <mergeCell ref="Q12:Q16"/>
     <mergeCell ref="P12:P16"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
     <mergeCell ref="D12:D16"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="M12:M16"/>
-    <mergeCell ref="N12:N16"/>
-    <mergeCell ref="O12:O16"/>
-    <mergeCell ref="L12:L16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="L17:L20"/>
+    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="N17:N20"/>
+    <mergeCell ref="O17:O20"/>
+    <mergeCell ref="P17:P20"/>
+    <mergeCell ref="Q17:Q20"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="C21:C26"/>
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="L21:L26"/>
+    <mergeCell ref="M21:M26"/>
+    <mergeCell ref="N21:N26"/>
+    <mergeCell ref="O21:O26"/>
+    <mergeCell ref="P21:P26"/>
+    <mergeCell ref="Q21:Q26"/>
+    <mergeCell ref="L27:L32"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="M27:M32"/>
+    <mergeCell ref="N27:N32"/>
+    <mergeCell ref="O27:O32"/>
+    <mergeCell ref="P27:P32"/>
+    <mergeCell ref="Q27:Q32"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I12:I37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I12:I32">
       <formula1>$I$9:$I$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -2824,11 +2621,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+    <sheetView zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
       <pane xSplit="5" ySplit="11" topLeftCell="F12" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22:A26"/>
+      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2894,13 +2691,13 @@
     </row>
     <row r="3" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="14"/>
@@ -3131,17 +2928,17 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="73">
+      <c r="A12" s="74">
         <v>1</v>
       </c>
-      <c r="B12" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="59" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="61" t="s">
-        <v>59</v>
+      <c r="B12" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="72" t="s">
+        <v>51</v>
       </c>
       <c r="E12" s="12">
         <v>1</v>
@@ -3149,7 +2946,7 @@
       <c r="F12" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="71" t="s">
+      <c r="G12" s="48" t="s">
         <v>34</v>
       </c>
       <c r="H12" s="24" t="s">
@@ -3164,43 +2961,43 @@
         <f t="shared" ref="K12" si="1">+IF(I12="OK",1,0)</f>
         <v>0</v>
       </c>
-      <c r="L12" s="51">
+      <c r="L12" s="55">
         <f>+(COUNTIF(J12:J16,1))</f>
         <v>0</v>
       </c>
-      <c r="M12" s="49">
+      <c r="M12" s="52">
         <f>+COUNT(E12:E16)</f>
         <v>5</v>
       </c>
-      <c r="N12" s="51">
+      <c r="N12" s="55">
         <f>+(COUNTIF(K12:K16,1))</f>
         <v>0</v>
       </c>
-      <c r="O12" s="53">
-        <v>0</v>
-      </c>
-      <c r="P12" s="57">
+      <c r="O12" s="58">
+        <v>0</v>
+      </c>
+      <c r="P12" s="61">
         <f>+L12/M12</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="57">
+      <c r="Q12" s="61">
         <f>+N12/M12</f>
         <v>0</v>
       </c>
       <c r="R12" s="38"/>
     </row>
     <row r="13" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="74"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="62"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="71"/>
       <c r="E13" s="1">
         <v>2</v>
       </c>
       <c r="F13" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="71" t="s">
+      <c r="G13" s="48" t="s">
         <v>34</v>
       </c>
       <c r="H13" s="11" t="s">
@@ -3209,19 +3006,19 @@
       <c r="I13" s="4"/>
       <c r="J13" s="40"/>
       <c r="K13" s="39"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="54"/>
-      <c r="P13" s="58"/>
-      <c r="Q13" s="58"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="62"/>
       <c r="R13" s="32"/>
     </row>
     <row r="14" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="74"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="62"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="71"/>
       <c r="E14" s="1">
         <v>3</v>
       </c>
@@ -3235,80 +3032,80 @@
       <c r="I14" s="4"/>
       <c r="J14" s="40"/>
       <c r="K14" s="39"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="58"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="62"/>
       <c r="R14" s="32"/>
     </row>
     <row r="15" spans="1:18" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="74"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="62"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="71"/>
       <c r="E15" s="1">
         <v>4</v>
       </c>
       <c r="F15" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="72" t="s">
+      <c r="G15" s="49" t="s">
         <v>37</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="4"/>
       <c r="J15" s="40"/>
       <c r="K15" s="39"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="54"/>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="58"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="62"/>
       <c r="R15" s="32"/>
     </row>
     <row r="16" spans="1:18" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="75"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
+      <c r="A16" s="76"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
       <c r="E16" s="5">
         <v>5</v>
       </c>
       <c r="F16" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="76" t="s">
+      <c r="G16" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="77" t="s">
-        <v>60</v>
+      <c r="H16" s="51" t="s">
+        <v>52</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="46"/>
       <c r="K16" s="43"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="65"/>
-      <c r="N16" s="64"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="67"/>
-      <c r="Q16" s="67"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="63"/>
       <c r="R16" s="47"/>
     </row>
     <row r="17" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="73">
+      <c r="A17" s="74">
         <v>2</v>
       </c>
-      <c r="B17" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="61" t="s">
-        <v>62</v>
+      <c r="B17" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="72" t="s">
+        <v>54</v>
       </c>
       <c r="E17" s="12">
         <v>1</v>
@@ -3316,7 +3113,7 @@
       <c r="F17" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="71" t="s">
+      <c r="G17" s="48" t="s">
         <v>34</v>
       </c>
       <c r="H17" s="24" t="s">
@@ -3331,43 +3128,43 @@
         <f t="shared" ref="K17" si="3">+IF(I17="OK",1,0)</f>
         <v>0</v>
       </c>
-      <c r="L17" s="51">
+      <c r="L17" s="55">
         <f>+(COUNTIF(J17:J21,1))</f>
         <v>0</v>
       </c>
-      <c r="M17" s="49">
+      <c r="M17" s="52">
         <f>+COUNT(E17:E21)</f>
         <v>5</v>
       </c>
-      <c r="N17" s="51">
+      <c r="N17" s="55">
         <f>+(COUNTIF(K17:K21,1))</f>
         <v>0</v>
       </c>
-      <c r="O17" s="53">
-        <v>0</v>
-      </c>
-      <c r="P17" s="57">
+      <c r="O17" s="58">
+        <v>0</v>
+      </c>
+      <c r="P17" s="61">
         <f>+L17/M17</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="57">
+      <c r="Q17" s="61">
         <f>+N17/M17</f>
         <v>0</v>
       </c>
       <c r="R17" s="38"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="74"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="62"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="1">
         <v>2</v>
       </c>
       <c r="F18" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="71" t="s">
+      <c r="G18" s="48" t="s">
         <v>34</v>
       </c>
       <c r="H18" s="11" t="s">
@@ -3376,19 +3173,19 @@
       <c r="I18" s="4"/>
       <c r="J18" s="40"/>
       <c r="K18" s="39"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="52"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="58"/>
-      <c r="Q18" s="58"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="59"/>
+      <c r="P18" s="62"/>
+      <c r="Q18" s="62"/>
       <c r="R18" s="32"/>
     </row>
     <row r="19" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="74"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="62"/>
+      <c r="A19" s="75"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="1">
         <v>3</v>
       </c>
@@ -3402,80 +3199,80 @@
       <c r="I19" s="4"/>
       <c r="J19" s="40"/>
       <c r="K19" s="39"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="52"/>
-      <c r="O19" s="54"/>
-      <c r="P19" s="58"/>
-      <c r="Q19" s="58"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="62"/>
       <c r="R19" s="32"/>
     </row>
     <row r="20" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="74"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="62"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="71"/>
       <c r="E20" s="1">
         <v>4</v>
       </c>
       <c r="F20" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="72" t="s">
+      <c r="G20" s="49" t="s">
         <v>37</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="4"/>
       <c r="J20" s="40"/>
       <c r="K20" s="39"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="52"/>
-      <c r="O20" s="54"/>
-      <c r="P20" s="58"/>
-      <c r="Q20" s="58"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="59"/>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="62"/>
       <c r="R20" s="32"/>
     </row>
     <row r="21" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="75"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
+      <c r="A21" s="76"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
       <c r="E21" s="5">
         <v>5</v>
       </c>
       <c r="F21" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="76" t="s">
+      <c r="G21" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="77" t="s">
-        <v>63</v>
+      <c r="H21" s="51" t="s">
+        <v>55</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="46"/>
       <c r="K21" s="43"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="65"/>
-      <c r="N21" s="64"/>
-      <c r="O21" s="66"/>
-      <c r="P21" s="67"/>
-      <c r="Q21" s="67"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="60"/>
+      <c r="P21" s="63"/>
+      <c r="Q21" s="63"/>
       <c r="R21" s="47"/>
     </row>
     <row r="22" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73">
+      <c r="A22" s="74">
         <v>3</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="72" t="s">
         <v>57</v>
-      </c>
-      <c r="C22" s="59" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="61" t="s">
-        <v>65</v>
       </c>
       <c r="E22" s="12">
         <v>1</v>
@@ -3483,7 +3280,7 @@
       <c r="F22" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="71" t="s">
+      <c r="G22" s="48" t="s">
         <v>34</v>
       </c>
       <c r="H22" s="24" t="s">
@@ -3498,43 +3295,43 @@
         <f t="shared" ref="K22" si="5">+IF(I22="OK",1,0)</f>
         <v>0</v>
       </c>
-      <c r="L22" s="51">
+      <c r="L22" s="55">
         <f>+(COUNTIF(J22:J26,1))</f>
         <v>0</v>
       </c>
-      <c r="M22" s="49">
+      <c r="M22" s="52">
         <f>+COUNT(E22:E26)</f>
         <v>5</v>
       </c>
-      <c r="N22" s="51">
+      <c r="N22" s="55">
         <f>+(COUNTIF(K22:K26,1))</f>
         <v>0</v>
       </c>
-      <c r="O22" s="53">
-        <v>0</v>
-      </c>
-      <c r="P22" s="57">
+      <c r="O22" s="58">
+        <v>0</v>
+      </c>
+      <c r="P22" s="61">
         <f>+L22/M22</f>
         <v>0</v>
       </c>
-      <c r="Q22" s="57">
+      <c r="Q22" s="61">
         <f>+N22/M22</f>
         <v>0</v>
       </c>
       <c r="R22" s="38"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="74"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="62"/>
+      <c r="A23" s="75"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="71"/>
       <c r="E23" s="1">
         <v>2</v>
       </c>
       <c r="F23" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G23" s="71" t="s">
+      <c r="G23" s="48" t="s">
         <v>34</v>
       </c>
       <c r="H23" s="11" t="s">
@@ -3543,19 +3340,19 @@
       <c r="I23" s="4"/>
       <c r="J23" s="40"/>
       <c r="K23" s="39"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="58"/>
-      <c r="Q23" s="58"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="59"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="62"/>
       <c r="R23" s="32"/>
     </row>
     <row r="24" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="74"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="62"/>
+      <c r="A24" s="75"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="71"/>
       <c r="E24" s="1">
         <v>3</v>
       </c>
@@ -3569,70 +3366,85 @@
       <c r="I24" s="4"/>
       <c r="J24" s="40"/>
       <c r="K24" s="39"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="54"/>
-      <c r="P24" s="58"/>
-      <c r="Q24" s="58"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="59"/>
+      <c r="P24" s="62"/>
+      <c r="Q24" s="62"/>
       <c r="R24" s="32"/>
     </row>
     <row r="25" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="74"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="62"/>
+      <c r="A25" s="75"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="71"/>
       <c r="E25" s="1">
         <v>4</v>
       </c>
       <c r="F25" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G25" s="72" t="s">
+      <c r="G25" s="49" t="s">
         <v>37</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="4"/>
       <c r="J25" s="40"/>
       <c r="K25" s="39"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="52"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="58"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="62"/>
       <c r="R25" s="32"/>
     </row>
     <row r="26" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="75"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
+      <c r="A26" s="76"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
       <c r="E26" s="5">
         <v>5</v>
       </c>
       <c r="F26" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="G26" s="76" t="s">
+      <c r="G26" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="H26" s="77" t="s">
-        <v>66</v>
+      <c r="H26" s="51" t="s">
+        <v>58</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="46"/>
       <c r="K26" s="43"/>
-      <c r="L26" s="64"/>
-      <c r="M26" s="65"/>
-      <c r="N26" s="64"/>
-      <c r="O26" s="66"/>
-      <c r="P26" s="67"/>
-      <c r="Q26" s="67"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="63"/>
       <c r="R26" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="M12:M16"/>
+    <mergeCell ref="N12:N16"/>
+    <mergeCell ref="O12:O16"/>
+    <mergeCell ref="P12:P16"/>
+    <mergeCell ref="Q12:Q16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="L12:L16"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="D17:D21"/>
     <mergeCell ref="Q17:Q21"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="B22:B26"/>
@@ -3649,21 +3461,6 @@
     <mergeCell ref="N17:N21"/>
     <mergeCell ref="O17:O21"/>
     <mergeCell ref="P17:P21"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="Q12:Q16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="L12:L16"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="M12:M16"/>
-    <mergeCell ref="N12:N16"/>
-    <mergeCell ref="O12:O16"/>
-    <mergeCell ref="P12:P16"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>